<commit_message>
Real data testing and fixing added
</commit_message>
<xml_diff>
--- a/validation_components/tests/fake_manifest2.xlsx
+++ b/validation_components/tests/fake_manifest2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cn14/manifest-validator/validation_components/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4BB6D5-BF17-7D45-8EE9-FE964DEFDBDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B804DF4-CFF1-9347-B12B-72D08F0F2E1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{005F83B0-C688-F640-A1E7-934BF66A365C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>SANGER PLATE ID</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>plate6</t>
+  </si>
+  <si>
+    <t>SUPPLIER SAMPLE NAME</t>
   </si>
 </sst>
 </file>
@@ -413,12 +416,13 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
@@ -427,6 +431,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -435,7 +442,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -446,7 +453,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="E3">
@@ -454,12 +461,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
@@ -467,7 +474,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
@@ -478,7 +485,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">

</xml_diff>

<commit_message>
Re-worked to use modular error message creation and includes manifests for testing
</commit_message>
<xml_diff>
--- a/validation_components/tests/fake_manifest2.xlsx
+++ b/validation_components/tests/fake_manifest2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cn14/manifest-validator/validation_components/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B804DF4-CFF1-9347-B12B-72D08F0F2E1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F2236A-CE04-394D-B8A6-A99A562075BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{005F83B0-C688-F640-A1E7-934BF66A365C}"/>
+    <workbookView xWindow="4100" yWindow="-20880" windowWidth="13900" windowHeight="16500" xr2:uid="{005F83B0-C688-F640-A1E7-934BF66A365C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>SANGER PLATE ID</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>SUPPLIER SAMPLE NAME</t>
+  </si>
+  <si>
+    <t>123dgfg</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,8 +494,8 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
-        <v>123456</v>
+      <c r="E8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>